<commit_message>
Tableau de Bord Manager Assistante et Synthese
</commit_message>
<xml_diff>
--- a/DOCS/Jeux de données.xlsx
+++ b/DOCS/Jeux de données.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1701871\Documents\GTA\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967C3932-7827-4AB3-8ADE-5D3004D07ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFCB8FF-E2DD-4787-B9FE-77B61AC20667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="données" sheetId="1" r:id="rId1"/>
@@ -5409,8 +5409,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5681,11 +5681,11 @@
         <v>2</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" ref="C23:C34" si="2">"insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values("&amp;A23&amp;","&amp;B23&amp;");"</f>
-        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(2,1);</v>
+        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(2,2);</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -5703,11 +5703,11 @@
         <v>2</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="2"/>
-        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(2,2);</v>
+        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(2,3);</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -5725,11 +5725,11 @@
         <v>3</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="2"/>
-        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(3,6);</v>
+        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(3,7);</v>
       </c>
       <c r="F25">
         <v>2</v>
@@ -5747,11 +5747,11 @@
         <v>4</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="2"/>
-        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(4,1);</v>
+        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(4,2);</v>
       </c>
       <c r="F26">
         <v>3</v>
@@ -5769,11 +5769,11 @@
         <v>4</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="2"/>
-        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(4,2);</v>
+        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(4,3);</v>
       </c>
       <c r="F27">
         <v>4</v>
@@ -5791,11 +5791,11 @@
         <v>4</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="2"/>
-        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(4,3);</v>
+        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(4,4);</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -5803,11 +5803,11 @@
         <v>4</v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="2"/>
-        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(4,4);</v>
+        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(4,5);</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -5815,11 +5815,11 @@
         <v>4</v>
       </c>
       <c r="B30">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="2"/>
-        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(4,5);</v>
+        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(4,6);</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -5827,11 +5827,11 @@
         <v>5</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="2"/>
-        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(5,4);</v>
+        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(5,5);</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>1151</v>
@@ -5842,11 +5842,11 @@
         <v>6</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="2"/>
-        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(6,2);</v>
+        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(6,3);</v>
       </c>
       <c r="F32" s="86">
         <v>1</v>
@@ -5864,11 +5864,11 @@
         <v>6</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="2"/>
-        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(6,3);</v>
+        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(6,4);</v>
       </c>
       <c r="F33" s="86">
         <v>2</v>
@@ -5886,11 +5886,11 @@
         <v>6</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="2"/>
-        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(6,4);</v>
+        <v>insert into gta_ActivitesParTypes (idTypePrestation,idActivite) values(6,5);</v>
       </c>
       <c r="F34" s="86">
         <v>3</v>
@@ -10902,8 +10902,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:U239"/>
   <sheetViews>
-    <sheetView topLeftCell="K18" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22350,7 +22350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E224D1D7-F57F-44CB-9CCB-B6AFB84720E2}">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>